<commit_message>
Cập nhật database mới
</commit_message>
<xml_diff>
--- a/mau_nhap_hocsinh.xlsx
+++ b/mau_nhap_hocsinh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>stt</t>
   </si>
@@ -47,7 +47,13 @@
     <t>dia_chi</t>
   </si>
   <si>
-    <t>lop</t>
+    <t>ngay_het_han_bhyt</t>
+  </si>
+  <si>
+    <t>ngay_het_han_bhtn</t>
+  </si>
+  <si>
+    <t>lop_hoc</t>
   </si>
   <si>
     <t>sdt_lienhe</t>
@@ -56,7 +62,16 @@
     <t>so_dinh_danh</t>
   </si>
   <si>
+    <t>noi_kham_bhyt</t>
+  </si>
+  <si>
     <t>ten_cha_me</t>
+  </si>
+  <si>
+    <t>doi_tuong_dong</t>
+  </si>
+  <si>
+    <t>ghi_chu</t>
   </si>
   <si>
     <t>ma_truong</t>
@@ -425,12 +440,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -557,7 +587,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -569,34 +599,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -681,24 +711,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1233,13 +1254,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="2.55555555555556" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.2222222222222" style="1" customWidth="1"/>
@@ -1247,14 +1268,19 @@
     <col min="4" max="4" width="11.5555555555556" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.7777777777778" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.2222222222222" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.2222222222222" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.8888888888889" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7777777777778" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7777777777778" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.4444444444444" style="1" customWidth="1"/>
     <col min="10" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88888888888889" style="1"/>
+    <col min="12" max="12" width="20.4444444444444" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7777777777778" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7777777777778" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6666666666667" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1288,58 +1314,21 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>